<commit_message>
New retrieval experiments, separated
</commit_message>
<xml_diff>
--- a/Recall/Recall_names.xlsx
+++ b/Recall/Recall_names.xlsx
@@ -5,17 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://lunduniversityo365-my.sharepoint.com/personal/pi6342kl_lu_se/Documents/Biofinder/fMRI-tasks/FacesNamesProfessions_fMRI/Recall/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hassl\OneDrive - Lund University\Biofinder\fMRI-tasks\FacesNamesProfessions_fMRI\Recall\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="11_F25DC773A252ABDACC1048BC415F7C7A5ADE58F2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D7DD9E52-AB27-4C80-A020-5EC9507A2132}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{135858AC-35F5-43F9-89E8-2000A75FE82E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="76">
   <si>
     <t>StimFile</t>
   </si>
@@ -230,67 +230,40 @@
     <t>Images_Faces/O51.jpg</t>
   </si>
   <si>
-    <t>Simon</t>
-  </si>
-  <si>
     <t>Images_Faces/O52.jpg</t>
   </si>
   <si>
-    <t>Håkan</t>
-  </si>
-  <si>
     <t>Images_Faces/O53.jpg</t>
   </si>
   <si>
-    <t>Christoffer</t>
-  </si>
-  <si>
     <t>Images_Faces/O54.jpg</t>
   </si>
   <si>
-    <t>Rickard</t>
-  </si>
-  <si>
     <t>Images_Faces/O55.jpg</t>
   </si>
   <si>
-    <t>Kjell</t>
-  </si>
-  <si>
     <t>Images_Faces/O56.jpg</t>
   </si>
   <si>
-    <t>William</t>
-  </si>
-  <si>
     <t>Images_Faces/O57.jpg</t>
   </si>
   <si>
-    <t>Joakim</t>
-  </si>
-  <si>
     <t>Images_Faces/O58.jpg</t>
   </si>
   <si>
-    <t>Stig</t>
-  </si>
-  <si>
     <t>Images_Faces/O59.jpg</t>
   </si>
   <si>
-    <t>Anton</t>
-  </si>
-  <si>
     <t>Images_Faces/O60.jpg</t>
   </si>
   <si>
-    <t>Wilhelm</t>
-  </si>
-  <si>
     <t>task</t>
   </si>
   <si>
     <t>Profession</t>
+  </si>
+  <si>
+    <t>NY</t>
   </si>
 </sst>
 </file>
@@ -354,10 +327,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -625,19 +594,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33:C41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="13.453125" customWidth="1"/>
     <col min="2" max="2" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -646,10 +615,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -663,7 +632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -677,7 +646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -691,7 +660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -705,7 +674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
@@ -719,7 +688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
@@ -733,7 +702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
@@ -747,7 +716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
@@ -761,7 +730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
@@ -775,7 +744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>2</v>
       </c>
@@ -789,7 +758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
@@ -803,7 +772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
@@ -817,7 +786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>2</v>
       </c>
@@ -831,7 +800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>2</v>
       </c>
@@ -845,7 +814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>2</v>
       </c>
@@ -859,7 +828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>2</v>
       </c>
@@ -873,7 +842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>2</v>
       </c>
@@ -887,7 +856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>2</v>
       </c>
@@ -901,7 +870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>2</v>
       </c>
@@ -915,7 +884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>2</v>
       </c>
@@ -929,7 +898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>2</v>
       </c>
@@ -943,7 +912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>2</v>
       </c>
@@ -957,7 +926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>2</v>
       </c>
@@ -971,7 +940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>2</v>
       </c>
@@ -985,7 +954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>2</v>
       </c>
@@ -999,7 +968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>2</v>
       </c>
@@ -1013,7 +982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>2</v>
       </c>
@@ -1027,7 +996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>2</v>
       </c>
@@ -1041,7 +1010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>2</v>
       </c>
@@ -1055,7 +1024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>2</v>
       </c>
@@ -1069,7 +1038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>2</v>
       </c>
@@ -1077,133 +1046,133 @@
         <v>63</v>
       </c>
       <c r="C32" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A33" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B33" t="s">
         <v>64</v>
       </c>
-      <c r="D32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
+        <v>75</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A34" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B34" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C34" t="s">
+        <v>75</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A35" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B35" t="s">
         <v>66</v>
       </c>
-      <c r="D33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B34" s="3" t="s">
+      <c r="C35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A36" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B36" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C36" t="s">
+        <v>75</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A37" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B37" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B35" t="s">
+      <c r="C37" t="s">
+        <v>75</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A38" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B38" t="s">
         <v>69</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C38" t="s">
+        <v>75</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A39" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B39" t="s">
         <v>70</v>
       </c>
-      <c r="D35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B36" s="3" t="s">
+      <c r="C39" t="s">
+        <v>75</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A40" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B40" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C40" t="s">
+        <v>75</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A41" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B41" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="D37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B38" t="s">
+      <c r="C41" t="s">
         <v>75</v>
-      </c>
-      <c r="C38" t="s">
-        <v>76</v>
-      </c>
-      <c r="D38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B39" t="s">
-        <v>77</v>
-      </c>
-      <c r="C39" t="s">
-        <v>78</v>
-      </c>
-      <c r="D39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="D40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>82</v>
       </c>
       <c r="D41">
         <v>0</v>

</xml_diff>